<commit_message>
Added Classification Report and Annotation Calc, fixed ambiguity Dataset
</commit_message>
<xml_diff>
--- a/Datasets/2nd Analysis Datasets/Excel/Ambiguity_Dataset.xlsx
+++ b/Datasets/2nd Analysis Datasets/Excel/Ambiguity_Dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\2nd Analysis Datasets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B7F991E-1FB8-4B96-98F4-C55FFDFCDAED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE420F3-ACA3-4209-A13E-B40A04D2F386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="3135" windowWidth="24240" windowHeight="17640" xr2:uid="{AB7D42DF-0837-483A-8BD4-3DC9231DE9A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{AB7D42DF-0837-483A-8BD4-3DC9231DE9A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +551,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>

</xml_diff>